<commit_message>
connexion à la base de données, corrections de bugs
</commit_message>
<xml_diff>
--- a/listDevices/Journal de bord.xlsx
+++ b/listDevices/Journal de bord.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
   <si>
     <t>Activité</t>
   </si>
@@ -63,18 +63,12 @@
     <t>J'ai encore cherché un peut pour trouvez une solution… sans résultats</t>
   </si>
   <si>
-    <t>Utilisation des htreads</t>
-  </si>
-  <si>
     <t>1h00</t>
   </si>
   <si>
     <t>J'ai décidé d'utiliser un thread qui allait s'occuper d'actualiser les clés USB branchées/débranchées. Comme ça on n'aura plus besoins d'actualiser l'affichage manuellement</t>
   </si>
   <si>
-    <t>MySQl</t>
-  </si>
-  <si>
     <t>J'ai recherché comment utilisé MySql en C#, j'en ai profiter pour installer Xampp j'ai eu quelques problèmes avec apache, visiblement les ports 80 et 443 étaient déjé utilisés j'ai donc remplacé les ports 80 par 8080 et 443 par 4433 dans apache.conf</t>
   </si>
   <si>
@@ -91,6 +85,21 @@
   </si>
   <si>
     <t>J'ai cherché une méthode pour afficher les ports des clés, j'ai trouvé un moyen de le faire en powerShell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J'ai chercher une solution pour récupérer les n° de ports et de hub, j'ai trouvé une librairie mais je n'ai pas réussi à l'utiliser </t>
+  </si>
+  <si>
+    <t>4h00</t>
+  </si>
+  <si>
+    <t>Utilisation des threads</t>
+  </si>
+  <si>
+    <t>2h30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J'ai corrigé les erreurs qui restaient par rapport à la connexion à la base de données, maintenant les enregistrement sont bien créer quand on insère une nouvelle clé, il ne reste plus qu'à mettre à jour les table si on change la clé de port </t>
   </si>
 </sst>
 </file>
@@ -409,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,16 +504,16 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1">
         <v>43501</v>
       </c>
       <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
         <v>15</v>
-      </c>
-      <c r="D6" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -518,26 +527,26 @@
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B8" s="1">
         <v>43501</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B9" s="1">
         <v>43501</v>
@@ -546,7 +555,35 @@
         <v>8</v>
       </c>
       <c r="D9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="1">
+        <v>43502</v>
+      </c>
+      <c r="C10" t="s">
         <v>23</v>
+      </c>
+      <c r="D10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="1">
+        <v>43503</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
récupération des emplacements des clés USB, mise à jour des tables
</commit_message>
<xml_diff>
--- a/listDevices/Journal de bord.xlsx
+++ b/listDevices/Journal de bord.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
   <si>
     <t>Activité</t>
   </si>
@@ -100,6 +100,24 @@
   </si>
   <si>
     <t xml:space="preserve">J'ai corrigé les erreurs qui restaient par rapport à la connexion à la base de données, maintenant les enregistrement sont bien créer quand on insère une nouvelle clé, il ne reste plus qu'à mettre à jour les table si on change la clé de port </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ports USB </t>
+  </si>
+  <si>
+    <t>3h00</t>
+  </si>
+  <si>
+    <t>Je n'ai définitvement trouvé aucun résultat pour récupérer les emplacements des clés en c#</t>
+  </si>
+  <si>
+    <t>J'ai décidé d'utiliser powerShell pour récupérer les ports des clés, j'ai trouvé un moyen d'exécuter un script en C# et d'en récupérer les informations</t>
+  </si>
+  <si>
+    <t>Debugage</t>
+  </si>
+  <si>
+    <t>Débugage de quelques bugs notamment en ce qui concernait la mise à jour des clés existantes</t>
   </si>
 </sst>
 </file>
@@ -418,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,6 +604,48 @@
         <v>26</v>
       </c>
     </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="1">
+        <v>43503</v>
+      </c>
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="1">
+        <v>43504</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="1">
+        <v>43504</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
mise à jour journal de bord
</commit_message>
<xml_diff>
--- a/listDevices/Journal de bord.xlsx
+++ b/listDevices/Journal de bord.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="50">
   <si>
     <t>Activité</t>
   </si>
@@ -148,6 +148,27 @@
   </si>
   <si>
     <t>J'ai continué de suivre le cours sur openclassroom je commence à comprendre comment fonctionne Laravel, je trouve ça vraiment intéressant</t>
+  </si>
+  <si>
+    <t>J'ai commencé à approché les bases de données avec laravel</t>
+  </si>
+  <si>
+    <t>Analyse du code de RackaKey</t>
+  </si>
+  <si>
+    <t>Analyse de code du projet RackaKey</t>
+  </si>
+  <si>
+    <t>Laravel et BDD</t>
+  </si>
+  <si>
+    <t>J'ai commencé à apprendre la façon dont laravel gère les bases de données, c'est assez complexe à comprendre</t>
+  </si>
+  <si>
+    <t>5h00</t>
+  </si>
+  <si>
+    <t>Je continue à apprendre comment utiliser les bases de données avec laravel</t>
   </si>
 </sst>
 </file>
@@ -466,17 +487,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="1" max="1" width="27" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" customWidth="1"/>
     <col min="4" max="4" width="114.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -746,6 +767,62 @@
         <v>42</v>
       </c>
     </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="1">
+        <v>43509</v>
+      </c>
+      <c r="C20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="1">
+        <v>43510</v>
+      </c>
+      <c r="C21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="1">
+        <v>43515</v>
+      </c>
+      <c r="C22" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="1">
+        <v>43516</v>
+      </c>
+      <c r="C23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" t="s">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>